<commit_message>
new commits batch run
</commit_message>
<xml_diff>
--- a/updated_vel_weight.xlsx
+++ b/updated_vel_weight.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaurangdada/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaurangdada/Downloads/FIDELITONE-Algorithm-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EDE8ADA-6B75-FB48-92CC-A908E6A95F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB31124-69ED-8541-9D13-A7384B54C324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1880" windowWidth="21680" windowHeight="16740" xr2:uid="{89D71C53-187F-4CDA-9638-8EB46AFEBC9C}"/>
+    <workbookView xWindow="10400" yWindow="460" windowWidth="21680" windowHeight="16740" xr2:uid="{89D71C53-187F-4CDA-9638-8EB46AFEBC9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Velocity + Weight" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="648">
   <si>
     <t>SKU ID</t>
   </si>
@@ -1929,13 +1929,88 @@
   </si>
   <si>
     <t>Z_Weight_scaled</t>
+  </si>
+  <si>
+    <t>CS56603</t>
+  </si>
+  <si>
+    <t>EA59121</t>
+  </si>
+  <si>
+    <t>CS58103</t>
+  </si>
+  <si>
+    <t>EA56410</t>
+  </si>
+  <si>
+    <t>CS61400</t>
+  </si>
+  <si>
+    <t>EA56103</t>
+  </si>
+  <si>
+    <t>CS56103</t>
+  </si>
+  <si>
+    <t>EA58510</t>
+  </si>
+  <si>
+    <t>CS57603</t>
+  </si>
+  <si>
+    <t>EA57610</t>
+  </si>
+  <si>
+    <t>CS61300</t>
+  </si>
+  <si>
+    <t>PKXX40#</t>
+  </si>
+  <si>
+    <t>CS58503</t>
+  </si>
+  <si>
+    <t>PK39226BAGr2</t>
+  </si>
+  <si>
+    <t>CS59503</t>
+  </si>
+  <si>
+    <t>CS57903</t>
+  </si>
+  <si>
+    <t>CS56403</t>
+  </si>
+  <si>
+    <t>EA59110</t>
+  </si>
+  <si>
+    <t>CS57103</t>
+  </si>
+  <si>
+    <t>EA57103</t>
+  </si>
+  <si>
+    <t>EA57110</t>
+  </si>
+  <si>
+    <t>CS56503</t>
+  </si>
+  <si>
+    <t>EA59510</t>
+  </si>
+  <si>
+    <t>CS59103</t>
+  </si>
+  <si>
+    <t>CS61100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1946,6 +2021,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1971,12 +2052,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2291,10 +2373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE58E107-8FC8-4708-810D-AFAF7932C1CE}">
-  <dimension ref="A1:N566"/>
+  <dimension ref="A1:N591"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+      <selection activeCell="G599" sqref="G599"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10118,7 +10200,7 @@
         <v>0.34</v>
       </c>
       <c r="G259">
-        <f t="shared" ref="G259:G322" si="8">C259+0.5306</f>
+        <f t="shared" ref="G259:G284" si="8">C259+0.5306</f>
         <v>1.0228603896333954E-4</v>
       </c>
       <c r="H259">
@@ -18377,6 +18459,481 @@
       <c r="H566">
         <f t="shared" si="13"/>
         <v>0.50407999999999997</v>
+      </c>
+    </row>
+    <row r="567" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A567" t="s">
+        <v>623</v>
+      </c>
+      <c r="B567" s="3">
+        <v>97</v>
+      </c>
+      <c r="C567">
+        <f>((B567 - L2)/L3)</f>
+        <v>-0.20386001355097763</v>
+      </c>
+      <c r="G567">
+        <f>C567+0.5306</f>
+        <v>0.32673998644902236</v>
+      </c>
+      <c r="H567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A568" t="s">
+        <v>624</v>
+      </c>
+      <c r="B568" s="3">
+        <v>82</v>
+      </c>
+      <c r="C568">
+        <f>((B568 - L2)/L3)</f>
+        <v>-0.25489715424004938</v>
+      </c>
+      <c r="G568">
+        <f t="shared" ref="G568:G591" si="14">C568+0.5306</f>
+        <v>0.27570284575995058</v>
+      </c>
+      <c r="H568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A569" t="s">
+        <v>625</v>
+      </c>
+      <c r="B569" s="3">
+        <v>48</v>
+      </c>
+      <c r="C569">
+        <f>((B569 - L2)/L3)</f>
+        <v>-0.37058133980194524</v>
+      </c>
+      <c r="G569">
+        <f t="shared" si="14"/>
+        <v>0.16001866019805472</v>
+      </c>
+      <c r="H569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A570" t="s">
+        <v>626</v>
+      </c>
+      <c r="B570" s="3">
+        <v>58</v>
+      </c>
+      <c r="C570">
+        <f>((B570 - L2)/L3)</f>
+        <v>-0.33655657934256411</v>
+      </c>
+      <c r="G570">
+        <f t="shared" si="14"/>
+        <v>0.19404342065743585</v>
+      </c>
+      <c r="H570">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A571" t="s">
+        <v>627</v>
+      </c>
+      <c r="B571" s="3">
+        <v>41</v>
+      </c>
+      <c r="C571">
+        <f>((B571 - L2)/L3)</f>
+        <v>-0.39439867212351204</v>
+      </c>
+      <c r="G571">
+        <f t="shared" si="14"/>
+        <v>0.13620132787648792</v>
+      </c>
+      <c r="H571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A572" t="s">
+        <v>628</v>
+      </c>
+      <c r="B572" s="3">
+        <v>18</v>
+      </c>
+      <c r="C572">
+        <f>((B72 - L2)/L3)</f>
+        <v>-6.4358495667514934E-2</v>
+      </c>
+      <c r="G572">
+        <f t="shared" si="14"/>
+        <v>0.46624150433248501</v>
+      </c>
+      <c r="H572">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A573" t="s">
+        <v>629</v>
+      </c>
+      <c r="B573" s="3">
+        <v>33</v>
+      </c>
+      <c r="C573">
+        <f>((B573 - L2)/L3)</f>
+        <v>-0.42161848049101697</v>
+      </c>
+      <c r="G573">
+        <f t="shared" si="14"/>
+        <v>0.10898151950898299</v>
+      </c>
+      <c r="H573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A574" t="s">
+        <v>630</v>
+      </c>
+      <c r="B574" s="3">
+        <v>73</v>
+      </c>
+      <c r="C574">
+        <f>((B574 - L2)/L3)</f>
+        <v>-0.28551943865349239</v>
+      </c>
+      <c r="G574">
+        <f t="shared" si="14"/>
+        <v>0.24508056134650757</v>
+      </c>
+      <c r="H574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A575" t="s">
+        <v>631</v>
+      </c>
+      <c r="B575" s="3">
+        <v>58</v>
+      </c>
+      <c r="C575">
+        <f>((B575 - L2)/L3)</f>
+        <v>-0.33655657934256411</v>
+      </c>
+      <c r="G575">
+        <f t="shared" si="14"/>
+        <v>0.19404342065743585</v>
+      </c>
+      <c r="H575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A576" t="s">
+        <v>632</v>
+      </c>
+      <c r="B576" s="3">
+        <v>134</v>
+      </c>
+      <c r="C576">
+        <f>((B576 - L2)/L3)</f>
+        <v>-7.7968399851267398E-2</v>
+      </c>
+      <c r="G576">
+        <f t="shared" si="14"/>
+        <v>0.45263160014873255</v>
+      </c>
+      <c r="H576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A577" t="s">
+        <v>633</v>
+      </c>
+      <c r="B577" s="3">
+        <v>29</v>
+      </c>
+      <c r="C577">
+        <f>((B577 - L2)/L3)</f>
+        <v>-0.43522838467476943</v>
+      </c>
+      <c r="G577">
+        <f t="shared" si="14"/>
+        <v>9.537161532523053E-2</v>
+      </c>
+      <c r="H577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A578" t="s">
+        <v>634</v>
+      </c>
+      <c r="B578" s="3">
+        <v>0</v>
+      </c>
+      <c r="C578">
+        <f>((B578 - L2)/L3)</f>
+        <v>-0.53390019000697475</v>
+      </c>
+      <c r="G578">
+        <f t="shared" si="14"/>
+        <v>-3.3001900069747903E-3</v>
+      </c>
+      <c r="H578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A579" t="s">
+        <v>635</v>
+      </c>
+      <c r="B579" s="3">
+        <v>16</v>
+      </c>
+      <c r="C579">
+        <f>((B579 - L2)/L3)</f>
+        <v>-0.47946057327196495</v>
+      </c>
+      <c r="G579">
+        <f t="shared" si="14"/>
+        <v>5.1139426728035009E-2</v>
+      </c>
+      <c r="H579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A580" t="s">
+        <v>636</v>
+      </c>
+      <c r="B580" s="3">
+        <v>0</v>
+      </c>
+      <c r="C580">
+        <f>((B580 - L2)/L3)</f>
+        <v>-0.53390019000697475</v>
+      </c>
+      <c r="G580">
+        <f t="shared" si="14"/>
+        <v>-3.3001900069747903E-3</v>
+      </c>
+      <c r="H580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A581" t="s">
+        <v>637</v>
+      </c>
+      <c r="B581" s="3">
+        <v>21</v>
+      </c>
+      <c r="C581">
+        <f>((B581 - L2)/L3)</f>
+        <v>-0.46244819304227436</v>
+      </c>
+      <c r="G581">
+        <f t="shared" si="14"/>
+        <v>6.8151806957725602E-2</v>
+      </c>
+      <c r="H581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A582" t="s">
+        <v>638</v>
+      </c>
+      <c r="B582" s="3">
+        <v>74</v>
+      </c>
+      <c r="C582">
+        <f>((B582- L2)/L3)</f>
+        <v>-0.28211696260755426</v>
+      </c>
+      <c r="G582">
+        <f t="shared" si="14"/>
+        <v>0.2484830373924457</v>
+      </c>
+      <c r="H582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A583" t="s">
+        <v>639</v>
+      </c>
+      <c r="B583" s="3">
+        <v>47</v>
+      </c>
+      <c r="C583">
+        <f>((B583 - L2)/L3)</f>
+        <v>-0.37398381584788337</v>
+      </c>
+      <c r="G583">
+        <f t="shared" si="14"/>
+        <v>0.15661618415211659</v>
+      </c>
+      <c r="H583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A584" t="s">
+        <v>640</v>
+      </c>
+      <c r="B584" s="3">
+        <v>85</v>
+      </c>
+      <c r="C584">
+        <f>((B584 - L2)/L3)</f>
+        <v>-0.24468972610223502</v>
+      </c>
+      <c r="G584">
+        <f t="shared" si="14"/>
+        <v>0.28591027389776491</v>
+      </c>
+      <c r="H584">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="585" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A585" t="s">
+        <v>641</v>
+      </c>
+      <c r="B585" s="3">
+        <v>58</v>
+      </c>
+      <c r="C585">
+        <f>((B585 - L2)/L3)</f>
+        <v>-0.33655657934256411</v>
+      </c>
+      <c r="G585">
+        <f t="shared" si="14"/>
+        <v>0.19404342065743585</v>
+      </c>
+      <c r="H585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A586" t="s">
+        <v>642</v>
+      </c>
+      <c r="B586" s="3">
+        <v>23</v>
+      </c>
+      <c r="C586">
+        <f>((B586 - L2)/L3)</f>
+        <v>-0.45564324095039815</v>
+      </c>
+      <c r="G586">
+        <f t="shared" si="14"/>
+        <v>7.4956759049601807E-2</v>
+      </c>
+      <c r="H586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A587" t="s">
+        <v>643</v>
+      </c>
+      <c r="B587" s="3">
+        <v>87</v>
+      </c>
+      <c r="C587">
+        <f>((B587 - L2)/L3)</f>
+        <v>-0.23788477401035879</v>
+      </c>
+      <c r="G587">
+        <f t="shared" si="14"/>
+        <v>0.29271522598964117</v>
+      </c>
+      <c r="H587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A588" t="s">
+        <v>644</v>
+      </c>
+      <c r="B588" s="3">
+        <v>68</v>
+      </c>
+      <c r="C588">
+        <f>((B588 - L2)/L3)</f>
+        <v>-0.30253181888318298</v>
+      </c>
+      <c r="G588">
+        <f t="shared" si="14"/>
+        <v>0.22806818111681698</v>
+      </c>
+      <c r="H588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A589" t="s">
+        <v>645</v>
+      </c>
+      <c r="B589" s="3">
+        <v>76</v>
+      </c>
+      <c r="C589">
+        <f>((B589 - L2)/L3)</f>
+        <v>-0.27531201051567805</v>
+      </c>
+      <c r="G589">
+        <f t="shared" si="14"/>
+        <v>0.25528798948432191</v>
+      </c>
+      <c r="H589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A590" t="s">
+        <v>646</v>
+      </c>
+      <c r="B590" s="3">
+        <v>25</v>
+      </c>
+      <c r="C590">
+        <f>((B590 - L2)/L3)</f>
+        <v>-0.44883828885852189</v>
+      </c>
+      <c r="G590">
+        <f t="shared" si="14"/>
+        <v>8.1761711141478066E-2</v>
+      </c>
+      <c r="H590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A591" t="s">
+        <v>647</v>
+      </c>
+      <c r="B591" s="3">
+        <v>41</v>
+      </c>
+      <c r="C591">
+        <f>((B591 - L2)/L3)</f>
+        <v>-0.39439867212351204</v>
+      </c>
+      <c r="G591">
+        <f t="shared" si="14"/>
+        <v>0.13620132787648792</v>
+      </c>
+      <c r="H591">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>